<commit_message>
Added complete experiment results
</commit_message>
<xml_diff>
--- a/results/batch_experiment.xlsx
+++ b/results/batch_experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/ITP_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1F4B4F-F915-E74D-BC37-F0BFD37E9647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1056232-B0C7-2C42-B8CA-353762232146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21520" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Removed 15" sheetId="9" r:id="rId1"/>
@@ -4527,6 +4527,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Variables affecting environmental sustainability</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7519,6 +7544,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Variables affecting social</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> benefit</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9000,6 +9055,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Variables</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> affecting economic profitability</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -39075,7 +39160,7 @@
         <v>10550</v>
       </c>
       <c r="O50">
-        <f t="shared" ref="O50:O81" si="15">SUM(K50:N50)</f>
+        <f t="shared" ref="O50:O72" si="15">SUM(K50:N50)</f>
         <v>167666</v>
       </c>
       <c r="P50">
@@ -39091,11 +39176,11 @@
         <v>35782</v>
       </c>
       <c r="T50">
-        <f t="shared" ref="T50:T81" si="16">SUM(P50:S50)</f>
+        <f t="shared" ref="T50:T72" si="16">SUM(P50:S50)</f>
         <v>95977</v>
       </c>
       <c r="U50">
-        <f t="shared" ref="U50:U81" si="17">O50+T50</f>
+        <f t="shared" ref="U50:U72" si="17">O50+T50</f>
         <v>263643</v>
       </c>
       <c r="V50">
@@ -39111,7 +39196,7 @@
         <v>12712074.155863101</v>
       </c>
       <c r="Z50">
-        <f t="shared" ref="Z50:Z81" si="18">Y50/AD50</f>
+        <f t="shared" ref="Z50:Z72" si="18">Y50/AD50</f>
         <v>3819.7338208723259</v>
       </c>
       <c r="AA50">
@@ -47155,7 +47240,7 @@
         <v>9111</v>
       </c>
       <c r="O114">
-        <f t="shared" ref="O114:O145" si="32">SUM(K114:N114)</f>
+        <f t="shared" ref="O114:O131" si="32">SUM(K114:N114)</f>
         <v>166190</v>
       </c>
       <c r="P114">
@@ -47171,11 +47256,11 @@
         <v>30359</v>
       </c>
       <c r="T114">
-        <f t="shared" ref="T114:T145" si="33">SUM(P114:S114)</f>
+        <f t="shared" ref="T114:T131" si="33">SUM(P114:S114)</f>
         <v>84645</v>
       </c>
       <c r="U114">
-        <f t="shared" ref="U114:U145" si="34">O114+T114</f>
+        <f t="shared" ref="U114:U131" si="34">O114+T114</f>
         <v>250835</v>
       </c>
       <c r="V114">
@@ -47191,7 +47276,7 @@
         <v>5971741.3645932702</v>
       </c>
       <c r="Z114">
-        <f t="shared" ref="Z114:Z145" si="35">Y114/AD114</f>
+        <f t="shared" ref="Z114:Z131" si="35">Y114/AD114</f>
         <v>5379.9471753092521</v>
       </c>
       <c r="AA114">
@@ -83701,8 +83786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36E41E6-2AFB-6B4C-8ABA-EFCA1E91B379}">
   <dimension ref="B2:AM263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D45" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K156" sqref="K156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding 3pg2py program to be used for validation
</commit_message>
<xml_diff>
--- a/results/batch_experiment.xlsx
+++ b/results/batch_experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/ITP_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1056232-B0C7-2C42-B8CA-353762232146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A52B71-A04A-BE42-A37F-38E63ADFBC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21520" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83786,8 +83786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36E41E6-2AFB-6B4C-8ABA-EFCA1E91B379}">
   <dimension ref="B2:AM263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D45" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K156" sqref="K156"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -83912,13 +83912,13 @@
         <v>49</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>29</v>
@@ -83940,14 +83940,14 @@
       <c r="F14">
         <v>0.88370000000000004</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
+        <v>3.1690000000000001E-4</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>0.53669999999999995</v>
-      </c>
-      <c r="H14" s="5">
-        <v>3.1690000000000001E-4</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
       </c>
       <c r="J14">
         <v>0.56459999999999999</v>
@@ -83970,13 +83970,13 @@
         <v>0.71499999999999997</v>
       </c>
       <c r="G15">
+        <v>0.89459999999999995</v>
+      </c>
+      <c r="H15">
+        <v>0.40150000000000002</v>
+      </c>
+      <c r="I15">
         <v>0.99539999999999995</v>
-      </c>
-      <c r="H15">
-        <v>0.89459999999999995</v>
-      </c>
-      <c r="I15">
-        <v>0.40150000000000002</v>
       </c>
       <c r="J15">
         <v>0.99770000000000003</v>
@@ -83998,14 +83998,14 @@
       <c r="F16" s="5">
         <v>6.4200000000000004E-3</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="7">
+        <v>5.4780000000000002E-3</v>
+      </c>
+      <c r="H16">
+        <v>0.2077</v>
+      </c>
+      <c r="I16" s="6">
         <v>2.0829999999999998E-6</v>
-      </c>
-      <c r="H16" s="7">
-        <v>5.4780000000000002E-3</v>
-      </c>
-      <c r="I16">
-        <v>0.2077</v>
       </c>
       <c r="J16" s="6">
         <v>3.8159999999999997E-15</v>
@@ -84027,14 +84027,14 @@
       <c r="F17" s="6">
         <v>1.5339999999999999E-5</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6">
+        <v>1.768E-5</v>
+      </c>
+      <c r="H17" s="6">
+        <v>9.8879999999999999E-12</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="H17" s="6">
-        <v>1.768E-5</v>
-      </c>
-      <c r="I17" s="6">
-        <v>9.8879999999999999E-12</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>50</v>
@@ -84056,14 +84056,14 @@
       <c r="F18" s="6">
         <v>6.6050000000000002E-12</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="9">
+        <v>6.5559999999999993E-2</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1.3340000000000001E-8</v>
+      </c>
+      <c r="I18">
         <v>0.89180000000000004</v>
-      </c>
-      <c r="H18" s="9">
-        <v>6.5559999999999993E-2</v>
-      </c>
-      <c r="I18" s="6">
-        <v>1.3340000000000001E-8</v>
       </c>
       <c r="J18">
         <v>0.97789999999999999</v>
@@ -84086,13 +84086,13 @@
         <v>9.4339999999999997E-3</v>
       </c>
       <c r="G19">
+        <v>0.94579999999999997</v>
+      </c>
+      <c r="H19">
+        <v>0.40150000000000002</v>
+      </c>
+      <c r="I19">
         <v>0.1268</v>
-      </c>
-      <c r="H19">
-        <v>0.94579999999999997</v>
-      </c>
-      <c r="I19">
-        <v>0.40150000000000002</v>
       </c>
       <c r="J19" s="6">
         <v>2.6010000000000002E-6</v>
@@ -84114,14 +84114,14 @@
       <c r="F20" s="5">
         <v>6.3889999999999997E-4</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="5">
+        <v>1.5949999999999999E-2</v>
+      </c>
+      <c r="H20">
+        <v>0.67510000000000003</v>
+      </c>
+      <c r="I20">
         <v>0.97399999999999998</v>
-      </c>
-      <c r="H20">
-        <v>1.5949999999999999E-2</v>
-      </c>
-      <c r="I20">
-        <v>0.67510000000000003</v>
       </c>
       <c r="J20">
         <v>0.38350000000000001</v>

</xml_diff>